<commit_message>
fixed pooling errors in llu
</commit_message>
<xml_diff>
--- a/documents/data.xlsx
+++ b/documents/data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="results" localSheetId="0">Sheet1!#REF!</definedName>
@@ -240,6 +241,351 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Normalized Compressed Cache Utilization for Benchmarks</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>POOLING</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$40:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$40:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.983472636477388</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.816733067729084</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>BASE-DELTA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$40:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$40:$G$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.873534375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.547253440995573</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.952191235059761</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BD+POOL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$40:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$40:$H$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.55078125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82782169197561</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.442231075697211</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2140568616"/>
+        <c:axId val="-2140838680"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2140568616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2140838680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2140838680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Normalized Compression Ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2140568616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.255686872633287"/>
+          <c:y val="0.882057349783149"/>
+          <c:w val="0.475267476107471"/>
+          <c:h val="0.0929872134967086"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -573,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1531,4 +1877,24 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>